<commit_message>
Final update before new implementation
Before implementing the new version where both RC depth and residuals are considered
</commit_message>
<xml_diff>
--- a/räls_livslängd/Wear/mistra_results.xlsx
+++ b/räls_livslängd/Wear/mistra_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbdouAA\Work Folders\Documents\GitHub\mistra-inframaint\räls_livslängd\Wear\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C40FF1D-0FC8-4A4D-A407-60E0E4BEA5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{350A1D3F-FD56-40DA-AB57-D40195F51154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" tabRatio="330" activeTab="3" xr2:uid="{3A71664D-9E65-4FDA-91B2-AC2A81079053}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="330" activeTab="3" xr2:uid="{3A71664D-9E65-4FDA-91B2-AC2A81079053}"/>
   </bookViews>
   <sheets>
     <sheet name="Wear" sheetId="1" r:id="rId1"/>
@@ -174,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,13 +188,68 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -206,14 +261,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bra" xfId="1" builtinId="26"/>
+    <cellStyle name="Dålig" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="75">
@@ -1227,9 +1297,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1267,7 +1337,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1373,7 +1443,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1515,7 +1585,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1526,7 +1596,7 @@
   <dimension ref="A5:AB40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD57"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,7 +1609,7 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
+      <c r="F5" s="7" t="s">
         <v>35</v>
       </c>
       <c r="V5" t="s">
@@ -1630,7 +1700,7 @@
       <c r="G7" t="s">
         <v>33</v>
       </c>
-      <c r="V7" t="s">
+      <c r="V7" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1712,22 +1782,22 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="H9">
@@ -1792,22 +1862,22 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>0.05</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>0.1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>0.11600000000000001</v>
       </c>
       <c r="H10">
@@ -1872,22 +1942,22 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="H11">
@@ -1952,22 +2022,22 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>6.3E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>7.8E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="H12">
@@ -2532,22 +2602,22 @@
       <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B29">
-        <v>0.53</v>
-      </c>
-      <c r="C29">
-        <v>0.53</v>
-      </c>
-      <c r="D29">
-        <v>0.53</v>
-      </c>
-      <c r="E29">
-        <v>0.53</v>
-      </c>
-      <c r="F29">
-        <v>0.53</v>
-      </c>
-      <c r="G29">
+      <c r="B29" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="G29" s="5">
         <v>0.53</v>
       </c>
       <c r="H29">
@@ -2612,22 +2682,22 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30">
-        <v>0.53</v>
-      </c>
-      <c r="C30">
-        <v>0.53</v>
-      </c>
-      <c r="D30">
-        <v>0.53</v>
-      </c>
-      <c r="E30">
-        <v>0.53</v>
-      </c>
-      <c r="F30">
-        <v>0.53</v>
-      </c>
-      <c r="G30">
+      <c r="B30" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="G30" s="5">
         <v>0.55000000000000004</v>
       </c>
       <c r="H30">
@@ -2692,22 +2762,22 @@
       <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B31">
-        <v>0.53</v>
-      </c>
-      <c r="C31">
-        <v>0.53</v>
-      </c>
-      <c r="D31">
-        <v>0.53</v>
-      </c>
-      <c r="E31">
-        <v>0.53</v>
-      </c>
-      <c r="F31">
-        <v>0.53</v>
-      </c>
-      <c r="G31">
+      <c r="B31" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="G31" s="5">
         <v>0.53</v>
       </c>
       <c r="H31">
@@ -2772,22 +2842,22 @@
       <c r="A32" t="s">
         <v>15</v>
       </c>
-      <c r="B32">
-        <v>0.53</v>
-      </c>
-      <c r="C32">
-        <v>0.53</v>
-      </c>
-      <c r="D32">
-        <v>0.53</v>
-      </c>
-      <c r="E32">
-        <v>0.53</v>
-      </c>
-      <c r="F32">
-        <v>0.53</v>
-      </c>
-      <c r="G32">
+      <c r="B32" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="G32" s="5">
         <v>0.53</v>
       </c>
       <c r="H32">
@@ -3199,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575556C3-9CD1-4D3F-93A7-9FEC3F5A934D}">
   <dimension ref="A6:AB39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3371,22 +3441,22 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="6">
         <v>1.03E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>2.3300000000000001E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>4.1099999999999998E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <v>5.3199999999999997E-2</v>
       </c>
       <c r="H9">
@@ -3451,22 +3521,22 @@
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="6">
         <v>1.24E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>2.07E-2</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>2.7E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>3.73E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>4.4699999999999997E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <v>5.5599999999999997E-2</v>
       </c>
       <c r="H10">
@@ -3531,22 +3601,22 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="6">
         <v>2.0899999999999998E-2</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>4.5499999999999999E-2</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="6">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
         <v>8.4699999999999998E-2</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="6">
         <v>0.1026</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="6">
         <v>0.1149</v>
       </c>
       <c r="H11">
@@ -3611,22 +3681,22 @@
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="6">
         <v>4.3799999999999999E-2</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="6">
         <v>9.9900000000000003E-2</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <v>0.12039999999999999</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>0.15260000000000001</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="6">
         <v>0.1842</v>
       </c>
       <c r="H12">
@@ -3853,22 +3923,22 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>3.4500000000000003E-2</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>5.28E-2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <v>7.2499999999999995E-2</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="6">
         <v>9.3100000000000002E-2</v>
       </c>
       <c r="H18">
@@ -3933,22 +4003,22 @@
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="6">
         <v>2.6100000000000002E-2</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="6">
         <v>5.5800000000000002E-2</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="6">
         <v>8.4599999999999995E-2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="6">
         <v>0.11650000000000001</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <v>0.14299999999999999</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="6">
         <v>0.1663</v>
       </c>
       <c r="H19">
@@ -4180,22 +4250,22 @@
       <c r="A29" t="s">
         <v>12</v>
       </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
         <v>0</v>
       </c>
       <c r="H29">
@@ -4260,22 +4330,22 @@
       <c r="A30" t="s">
         <v>13</v>
       </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
         <v>0</v>
       </c>
       <c r="H30">
@@ -4340,22 +4410,22 @@
       <c r="A31" t="s">
         <v>14</v>
       </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
         <v>0</v>
       </c>
       <c r="H31">
@@ -4420,22 +4490,22 @@
       <c r="A32" t="s">
         <v>15</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
         <v>0</v>
       </c>
       <c r="H32">
@@ -4667,22 +4737,22 @@
       <c r="A38" t="s">
         <v>14</v>
       </c>
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
         <v>0</v>
       </c>
       <c r="H38">
@@ -4747,22 +4817,22 @@
       <c r="A39" t="s">
         <v>15</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
+      <c r="B39" s="5">
+        <v>0</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
         <v>0</v>
       </c>
       <c r="H39">
@@ -4842,8 +4912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C240127D-17EB-4812-A2BA-3FDC0D42802F}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M9" sqref="A1:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4941,25 +5011,25 @@
       <c r="A3">
         <v>1440</v>
       </c>
-      <c r="B3">
-        <v>0.53</v>
-      </c>
-      <c r="C3">
-        <v>0.53</v>
-      </c>
-      <c r="D3">
-        <v>0.53</v>
-      </c>
-      <c r="E3">
-        <v>0.53</v>
-      </c>
-      <c r="F3">
-        <v>0.53</v>
-      </c>
-      <c r="G3">
-        <v>0.53</v>
-      </c>
-      <c r="H3">
+      <c r="B3" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H3" s="4">
         <v>0.74</v>
       </c>
       <c r="I3">
@@ -4982,25 +5052,25 @@
       <c r="A4">
         <v>1445</v>
       </c>
-      <c r="B4">
-        <v>0.53</v>
-      </c>
-      <c r="C4">
-        <v>0.53</v>
-      </c>
-      <c r="D4">
-        <v>0.53</v>
-      </c>
-      <c r="E4">
-        <v>0.53</v>
-      </c>
-      <c r="F4">
-        <v>0.53</v>
-      </c>
-      <c r="G4">
+      <c r="B4" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>0.89</v>
       </c>
       <c r="I4">
@@ -5023,32 +5093,32 @@
       <c r="A5">
         <v>1450</v>
       </c>
-      <c r="B5">
-        <v>0.53</v>
-      </c>
-      <c r="C5">
-        <v>0.53</v>
-      </c>
-      <c r="D5">
-        <v>0.53</v>
-      </c>
-      <c r="E5">
-        <v>0.53</v>
-      </c>
-      <c r="F5">
-        <v>0.53</v>
-      </c>
-      <c r="G5">
-        <v>0.53</v>
-      </c>
-      <c r="H5">
-        <v>0.74</v>
-      </c>
-      <c r="I5">
-        <v>0.88</v>
-      </c>
-      <c r="J5">
-        <v>0.89</v>
+      <c r="B5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.99</v>
       </c>
       <c r="K5">
         <v>1.03</v>
@@ -5064,25 +5134,25 @@
       <c r="A6">
         <v>1455</v>
       </c>
-      <c r="B6">
-        <v>0.53</v>
-      </c>
-      <c r="C6">
-        <v>0.53</v>
-      </c>
-      <c r="D6">
-        <v>0.53</v>
-      </c>
-      <c r="E6">
-        <v>0.53</v>
-      </c>
-      <c r="F6">
-        <v>0.53</v>
-      </c>
-      <c r="G6">
-        <v>0.53</v>
-      </c>
-      <c r="H6">
+      <c r="B6" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H6" s="4">
         <v>0.9</v>
       </c>
       <c r="I6">
@@ -5105,22 +5175,22 @@
       <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H7" t="s">
@@ -5146,28 +5216,28 @@
       <c r="A8">
         <v>1450</v>
       </c>
-      <c r="B8">
-        <v>0.53</v>
-      </c>
-      <c r="C8">
-        <v>0.53</v>
-      </c>
-      <c r="D8">
-        <v>0.53</v>
-      </c>
-      <c r="E8">
-        <v>0.53</v>
-      </c>
-      <c r="F8">
-        <v>0.53</v>
-      </c>
-      <c r="G8">
-        <v>0.53</v>
-      </c>
-      <c r="H8">
+      <c r="B8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H8" s="4">
         <v>0.78</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <v>0.88</v>
       </c>
       <c r="J8">
@@ -5187,35 +5257,35 @@
       <c r="A9">
         <v>1455</v>
       </c>
-      <c r="B9">
-        <v>0.53</v>
-      </c>
-      <c r="C9">
-        <v>0.53</v>
-      </c>
-      <c r="D9">
-        <v>0.53</v>
-      </c>
-      <c r="E9">
-        <v>0.53</v>
-      </c>
-      <c r="F9">
-        <v>0.53</v>
-      </c>
-      <c r="G9">
-        <v>0.53</v>
-      </c>
-      <c r="H9">
-        <v>0.7</v>
-      </c>
-      <c r="I9">
-        <v>0.86</v>
+      <c r="B9" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.88</v>
       </c>
       <c r="J9">
         <v>0.89</v>
       </c>
-      <c r="K9">
-        <v>0.94</v>
+      <c r="K9" s="9">
+        <v>0.96</v>
       </c>
       <c r="L9">
         <v>1.1000000000000001</v>
@@ -5236,8 +5306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CE4E5A-ADD0-4101-BB70-0C5E1C06C9B2}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5328,22 +5398,22 @@
       <c r="A3">
         <v>1440</v>
       </c>
-      <c r="B3" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="B3" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="G3" s="3">
         <v>0.53</v>
       </c>
       <c r="H3" s="1">
@@ -5369,22 +5439,22 @@
       <c r="A4">
         <v>1445</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="B4" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F4" s="3">
         <v>0.54</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
         <v>0.56999999999999995</v>
       </c>
       <c r="H4" s="1">
@@ -5410,22 +5480,22 @@
       <c r="A5">
         <v>1450</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="B5" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="G5" s="3">
         <v>0.53</v>
       </c>
       <c r="H5" s="1">
@@ -5451,26 +5521,26 @@
       <c r="A6">
         <v>1455</v>
       </c>
-      <c r="B6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="B6" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="G6" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H6" s="1">
-        <v>0.8</v>
+      <c r="H6" s="10">
+        <v>0.81</v>
       </c>
       <c r="I6" s="1">
         <v>0.91</v>
@@ -5533,22 +5603,22 @@
       <c r="A8">
         <v>1450</v>
       </c>
-      <c r="B8" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="B8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="G8" s="3">
         <v>0.53</v>
       </c>
       <c r="H8" s="1">
@@ -5574,22 +5644,22 @@
       <c r="A9">
         <v>1455</v>
       </c>
-      <c r="B9" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.53</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="B9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="G9" s="3">
         <v>0.53</v>
       </c>
       <c r="H9" s="1">

</xml_diff>